<commit_message>
Updated edit page, made the project's billable default for a log, updated the template file
</commit_message>
<xml_diff>
--- a/Templates/Template Hours Log.xlsx
+++ b/Templates/Template Hours Log.xlsx
@@ -1380,7 +1380,7 @@
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <dataValidations count="2">
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose your name from this list" sqref="A3">
-      <formula1>People!$A$2:$A$9</formula1>
+      <formula1>People!$A$2:$A$10</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose your starting date from this list" sqref="A6">
       <formula1>Dates!$A$2:$A$85</formula1>
@@ -3033,7 +3033,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B2">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E2">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3042,7 +3042,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B3">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E3">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3051,7 +3051,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B4">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E4">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3060,7 +3060,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B5">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E5">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3069,7 +3069,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B6">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E6">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3078,7 +3078,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B7">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E7">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3087,7 +3087,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B8">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E8">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3096,7 +3096,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B9">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E9">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3105,7 +3105,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B10">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E10">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3114,7 +3114,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B11">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E11">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3123,7 +3123,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B12">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E12">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3132,7 +3132,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B13">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E13">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3141,7 +3141,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B14">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E14">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3150,7 +3150,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B15">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E15">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3159,7 +3159,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B16">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E16">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3168,7 +3168,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B17">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E17">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3177,7 +3177,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B18">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E18">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3186,7 +3186,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B19">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E19">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3195,7 +3195,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B20">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E20">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3204,7 +3204,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B21">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E21">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3213,7 +3213,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B22">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E22">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3222,7 +3222,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B23">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E23">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3231,7 +3231,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B24">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E24">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3240,7 +3240,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B25">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E25">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3249,7 +3249,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B26">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E26">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3258,7 +3258,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B27">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E27">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3267,7 +3267,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B28">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E28">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3276,7 +3276,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B29">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E29">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3285,7 +3285,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B30">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E30">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3294,7 +3294,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B31">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E31">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3303,7 +3303,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B32">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E32">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3312,7 +3312,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B33">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E33">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3321,7 +3321,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B34">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E34">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3330,7 +3330,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B35">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E35">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3339,7 +3339,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B36">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E36">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3348,7 +3348,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B37">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E37">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3357,7 +3357,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B38">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E38">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3366,7 +3366,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B39">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E39">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3375,7 +3375,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B40">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E40">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3384,7 +3384,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B41">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E41">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3393,7 +3393,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B42">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E42">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3402,7 +3402,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B43">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E43">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3411,7 +3411,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B44">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E44">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3420,7 +3420,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B45">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E45">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3429,7 +3429,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B46">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E46">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3438,7 +3438,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B47">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E47">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3447,7 +3447,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B48">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E48">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3456,7 +3456,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B49">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E49">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3465,7 +3465,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B50">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E50">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3474,7 +3474,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B51">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E51">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3483,7 +3483,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B52">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E52">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3492,7 +3492,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B53">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E53">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3501,7 +3501,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B54">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E54">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3510,7 +3510,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B55">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E55">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3519,7 +3519,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B56">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E56">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3528,7 +3528,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B57">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E57">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3537,7 +3537,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B58">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E58">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3546,7 +3546,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B59">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E59">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3555,7 +3555,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B60">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E60">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3564,7 +3564,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B61">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E61">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3573,7 +3573,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B62">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E62">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3582,7 +3582,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B63">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E63">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3591,7 +3591,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B64">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E64">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3600,7 +3600,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B65">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E65">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3609,7 +3609,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B66">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E66">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3618,7 +3618,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B67">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E67">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3627,7 +3627,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B68">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E68">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3636,7 +3636,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B69">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E69">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3645,7 +3645,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B70">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E70">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3654,7 +3654,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B71">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E71">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3663,7 +3663,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B72">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E72">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3672,7 +3672,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B73">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E73">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3681,7 +3681,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B74">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E74">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3690,7 +3690,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B75">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E75">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3699,7 +3699,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B76">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E76">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3708,7 +3708,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B77">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E77">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3717,7 +3717,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B78">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E78">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3726,7 +3726,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B79">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E79">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3735,7 +3735,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B80">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E80">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3744,7 +3744,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B81">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E81">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3753,7 +3753,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B82">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E82">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3762,7 +3762,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B83">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E83">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3771,7 +3771,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B84">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E84">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3780,7 +3780,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B85">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E85">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3789,7 +3789,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B86">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E86">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3798,7 +3798,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B87">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E87">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3807,7 +3807,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B88">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E88">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3816,7 +3816,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B89">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E89">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3825,7 +3825,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B90">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E90">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3834,7 +3834,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B91">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E91">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3843,7 +3843,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B92">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E92">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3852,7 +3852,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B93">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E93">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3861,7 +3861,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B94">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E94">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3870,7 +3870,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B95">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E95">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3879,7 +3879,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B96">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E96">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3888,7 +3888,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B97">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E97">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3897,7 +3897,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B98">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E98">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3906,7 +3906,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B99">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E99">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3915,7 +3915,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B100">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E100">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3924,7 +3924,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B101">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E101">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3933,7 +3933,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B102">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E102">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3942,7 +3942,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B103">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E103">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3951,7 +3951,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B104">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E104">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3960,7 +3960,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B105">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E105">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3969,7 +3969,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B106">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E106">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3978,7 +3978,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B107">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E107">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3987,7 +3987,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B108">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E108">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -3996,7 +3996,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B109">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E109">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4005,7 +4005,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B110">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E110">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4014,7 +4014,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B111">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E111">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4023,7 +4023,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B112">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E112">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4032,7 +4032,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B113">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E113">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4041,7 +4041,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B114">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E114">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4050,7 +4050,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B115">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E115">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4059,7 +4059,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B116">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E116">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4068,7 +4068,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B117">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E117">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4077,7 +4077,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B118">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E118">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4086,7 +4086,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B119">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E119">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4095,7 +4095,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B120">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E120">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4104,7 +4104,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B121">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E121">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4113,7 +4113,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B122">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E122">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4122,7 +4122,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B123">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E123">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4131,7 +4131,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B124">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E124">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4140,7 +4140,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B125">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E125">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4149,7 +4149,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B126">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E126">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4158,7 +4158,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B127">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E127">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4167,7 +4167,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B128">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E128">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4176,7 +4176,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B129">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E129">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4185,7 +4185,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B130">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E130">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4194,7 +4194,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B131">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E131">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4203,7 +4203,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B132">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E132">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4212,7 +4212,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B133">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E133">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4221,7 +4221,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B134">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E134">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4230,7 +4230,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B135">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E135">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4239,7 +4239,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B136">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E136">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4248,7 +4248,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B137">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E137">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4257,7 +4257,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B138">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E138">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4266,7 +4266,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B139">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E139">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4275,7 +4275,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B140">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E140">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4284,7 +4284,7 @@
       <formula1>Name!$A$6:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="B141">
-      <formula1>Projects!$A$2:$A$141</formula1>
+      <formula1>Projects!$A$2:$A$142</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick Yes or No" sqref="E141">
       <formula1>'Validation Lists'!$A$2:$A$3</formula1>
@@ -4309,7 +4309,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D141"/>
+  <dimension ref="A1:D142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A2" sqref="A2"/>
@@ -4578,25 +4578,25 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C27"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="C28"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29" t="s">
         <v>36</v>
@@ -4605,7 +4605,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
         <v>36</v>
@@ -4614,16 +4614,16 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C31"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
         <v>12</v>
@@ -4632,7 +4632,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B33" t="s">
         <v>12</v>
@@ -4641,7 +4641,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
         <v>12</v>
@@ -4650,7 +4650,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
         <v>12</v>
@@ -4659,7 +4659,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
         <v>12</v>
@@ -4668,7 +4668,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
         <v>12</v>
@@ -4677,63 +4677,63 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="C38"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C39"/>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" t="s">
-        <v>60</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C40"/>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B41" t="s">
-        <v>12</v>
-      </c>
-      <c r="C41"/>
+        <v>38</v>
+      </c>
+      <c r="C41" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B42" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="C42"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C43"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B44" t="s">
         <v>38</v>
@@ -4742,25 +4742,25 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="C45"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B46" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="C46"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B47" t="s">
         <v>12</v>
@@ -4769,7 +4769,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B48" t="s">
         <v>12</v>
@@ -4778,16 +4778,16 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B49" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C49"/>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B50" t="s">
         <v>20</v>
@@ -4796,7 +4796,7 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B51" t="s">
         <v>20</v>
@@ -4805,7 +4805,7 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B52" t="s">
         <v>20</v>
@@ -4814,25 +4814,25 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B53" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="C53"/>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B54" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="C54"/>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B55" t="s">
         <v>12</v>
@@ -4841,7 +4841,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B56" t="s">
         <v>12</v>
@@ -4850,25 +4850,25 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B57" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="C57"/>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B58" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C58"/>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B59" t="s">
         <v>12</v>
@@ -4877,7 +4877,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B60" t="s">
         <v>12</v>
@@ -4886,54 +4886,54 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B61" t="s">
-        <v>83</v>
-      </c>
-      <c r="C61" t="s">
-        <v>84</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C61"/>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B62" t="s">
-        <v>38</v>
-      </c>
-      <c r="C62"/>
+        <v>83</v>
+      </c>
+      <c r="C62" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B63" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C63"/>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B64" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="C64"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B65" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="C65"/>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B66" t="s">
         <v>38</v>
@@ -4942,7 +4942,7 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B67" t="s">
         <v>38</v>
@@ -4951,19 +4951,23 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
+        <v>90</v>
+      </c>
+      <c r="B68" t="s">
+        <v>38</v>
+      </c>
+      <c r="C68"/>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
         <v>91</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>20</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C69" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69"/>
-      <c r="B69"/>
-      <c r="C69"/>
     </row>
     <row r="70" spans="1:4">
       <c r="A70"/>
@@ -5325,988 +5329,1000 @@
       <c r="B141"/>
       <c r="C141"/>
     </row>
+    <row r="142" spans="1:4">
+      <c r="A142"/>
+      <c r="B142"/>
+      <c r="C142"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <dataValidations count="280">
+  <dataValidations count="282">
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C2">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B2">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B3">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C3">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B4">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C4">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B5">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C5">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B6">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C6">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B7">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C7">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B8">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C8">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B9">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C9">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B10">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C10">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B11">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C11">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B12">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C12">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B13">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C13">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B14">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C14">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B15">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C15">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B16">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C16">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B17">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C17">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B18">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C18">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B19">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C19">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B20">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C20">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B21">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C21">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B22">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C22">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B23">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C23">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B24">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C24">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B25">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C25">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B26">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C26">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C142">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B142">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C141">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B141">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C140">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B140">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C139">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B139">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C138">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B138">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C137">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B137">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C136">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B136">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C135">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B135">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C134">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B134">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C133">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B133">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C132">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B132">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C131">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B131">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C130">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B130">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C129">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B129">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C128">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B128">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C127">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B127">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C126">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B126">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C125">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B125">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C124">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B124">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C123">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B123">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C122">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B122">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C121">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B121">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C120">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B120">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C119">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B119">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C118">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B118">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C117">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B117">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C116">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B116">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C115">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B115">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C114">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B114">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C113">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B113">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C112">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B112">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C111">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B111">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C110">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B110">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C109">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B109">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C108">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B108">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C107">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B107">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C106">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B106">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C105">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B105">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C104">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B104">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C103">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B103">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C102">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B102">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C101">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B101">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C100">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B100">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C99">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B99">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C98">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B98">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C97">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B97">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C96">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B96">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C95">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B95">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C94">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B94">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C93">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B93">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C92">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B92">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C91">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B91">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C90">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B90">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C89">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B89">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C88">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B88">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C87">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B87">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C86">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B86">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C85">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B85">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C84">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B84">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C83">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B83">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C82">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B82">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C81">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B81">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C80">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B80">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C79">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B79">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C78">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B78">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C77">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B77">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C76">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B76">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C75">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B75">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C74">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B74">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C73">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B73">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C72">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B72">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C71">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B71">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C70">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B70">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C69">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B69">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C68">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B68">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C67">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B67">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C66">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B66">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C65">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B65">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C64">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B64">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C63">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B63">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C62">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B62">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C61">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B61">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C60">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B60">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C59">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B59">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C58">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B58">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C57">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B57">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C56">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B56">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C55">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B55">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C54">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B54">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C53">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B53">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C52">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B52">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C51">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B51">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C50">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B50">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C49">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B49">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C48">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B48">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C47">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B47">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C46">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B46">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C45">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B45">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C44">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B44">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C43">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B43">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C42">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B42">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C41">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B41">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C40">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B40">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C39">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B39">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C38">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B38">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C37">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B37">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C36">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B36">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C35">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B35">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C34">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B34">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C33">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B33">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C32">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B32">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C31">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B31">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C30">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B30">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C29">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B29">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C28">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B28">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C27">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B27">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C27">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B28">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C28">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B29">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C29">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B30">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C30">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B31">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C31">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B32">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C32">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B33">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C33">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B34">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C34">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B35">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C35">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B36">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C36">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B37">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C37">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B38">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C38">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B39">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C39">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B40">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C40">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B41">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C41">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B42">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C42">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B43">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C43">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B44">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C44">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B45">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C45">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B46">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C46">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B47">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C47">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B48">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C48">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B49">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C49">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B50">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C50">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B51">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C51">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B52">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C52">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B53">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C53">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B54">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C54">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B55">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C55">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B56">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C56">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B57">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C57">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B58">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C58">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B59">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C59">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B60">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C60">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B61">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C61">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B62">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C62">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B63">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C63">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B64">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C64">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B65">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C65">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B66">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C66">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B67">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C67">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B68">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C68">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B69">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C69">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B70">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C70">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B71">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C71">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B72">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C72">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B73">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C73">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B74">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C74">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B75">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C75">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B76">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C76">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B77">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C77">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B78">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C78">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B79">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C79">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B80">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C80">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B81">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C81">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B82">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C82">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B83">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C83">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B84">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C84">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B85">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C85">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B86">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C86">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B87">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C87">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B88">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C88">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B89">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C89">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B90">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C90">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B91">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C91">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B92">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C92">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B93">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C93">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B94">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C94">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B95">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C95">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B96">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C96">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B97">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C97">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B98">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C98">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B99">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C99">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B100">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C100">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B101">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C101">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B102">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C102">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B103">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C103">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B104">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C104">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B105">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C105">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B106">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C106">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B107">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C107">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B108">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C108">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B109">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C109">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B110">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C110">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B111">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C111">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B112">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C112">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B113">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C113">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B114">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C114">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B115">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C115">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B116">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C116">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B117">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C117">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B118">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C118">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B119">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C119">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B120">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C120">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B121">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C121">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B122">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C122">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B123">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C123">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B124">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C124">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B125">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C125">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B126">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C126">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B127">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C127">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B128">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C128">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B129">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C129">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B130">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C130">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B131">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C131">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B132">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C132">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B133">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C133">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B134">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C134">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B135">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C135">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B136">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C136">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B137">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C137">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B138">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C138">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B139">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C139">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B140">
-      <formula1>Categories!$C$2:$C$11</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C140">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C141">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B141">
-      <formula1>Categories!$C$2:$C$11</formula1>
+      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions gridLines="false" gridLinesSet="true"/>
@@ -6328,7 +6344,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="B12" sqref="B12"/>
@@ -6361,43 +6377,82 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B4"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>83</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B5"/>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>36</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B7"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>20</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="B9"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>38</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B10"/>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
         <v>87</v>
       </c>
+      <c r="B17"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -6420,7 +6475,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A8" sqref="A8"/>
@@ -6468,11 +6523,16 @@
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed a number of errors in the code related to setting default time zone as well as other issues.
</commit_message>
<xml_diff>
--- a/Templates/Template Hours Log.xlsx
+++ b/Templates/Template Hours Log.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="109">
   <si>
     <t>Time Report</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>Custom Services - Consulting and Training</t>
-  </si>
-  <si>
-    <t>Subcontract to David Evans Associates - DEA for scenario planning for BTPO</t>
   </si>
   <si>
     <t>Boston College ITEST</t>
@@ -4343,14 +4340,12 @@
       <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="C2" s="2"/>
       <c r="D2"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -4359,18 +4354,18 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -4379,7 +4374,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -4388,206 +4383,206 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
       </c>
       <c r="C7"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
         <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
         <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
       </c>
       <c r="C19"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s">
         <v>37</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>38</v>
-      </c>
-      <c r="C20" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" t="s">
         <v>43</v>
-      </c>
-      <c r="B24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26"/>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
@@ -4596,34 +4591,34 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C29"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C31"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B32" t="s">
         <v>12</v>
@@ -4632,7 +4627,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B33" t="s">
         <v>12</v>
@@ -4641,7 +4636,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B34" t="s">
         <v>12</v>
@@ -4650,7 +4645,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
         <v>12</v>
@@ -4659,7 +4654,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36" t="s">
         <v>12</v>
@@ -4668,7 +4663,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B37" t="s">
         <v>12</v>
@@ -4677,7 +4672,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B38" t="s">
         <v>12</v>
@@ -4686,36 +4681,36 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C39"/>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C40"/>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" t="s">
         <v>59</v>
-      </c>
-      <c r="B41" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B42" t="s">
         <v>12</v>
@@ -4724,43 +4719,43 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C43"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C44"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C45"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
+        <v>64</v>
+      </c>
+      <c r="B46" t="s">
         <v>65</v>
-      </c>
-      <c r="B46" t="s">
-        <v>66</v>
       </c>
       <c r="C46"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B47" t="s">
         <v>12</v>
@@ -4769,7 +4764,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B48" t="s">
         <v>12</v>
@@ -4778,7 +4773,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B49" t="s">
         <v>12</v>
@@ -4787,52 +4782,52 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B50" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C50"/>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C51"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C52"/>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C53"/>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C54"/>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B55" t="s">
         <v>12</v>
@@ -4841,7 +4836,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B56" t="s">
         <v>12</v>
@@ -4850,7 +4845,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B57" t="s">
         <v>12</v>
@@ -4859,16 +4854,16 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B58" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C58"/>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B59" t="s">
         <v>12</v>
@@ -4877,7 +4872,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B60" t="s">
         <v>12</v>
@@ -4886,7 +4881,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B61" t="s">
         <v>12</v>
@@ -4895,27 +4890,27 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
+        <v>81</v>
+      </c>
+      <c r="B62" t="s">
         <v>82</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>83</v>
-      </c>
-      <c r="C62" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B63" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C63"/>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B64" t="s">
         <v>12</v>
@@ -4924,49 +4919,49 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B65" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C65"/>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B66" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C66"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B67" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C67"/>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B68" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C68"/>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
+        <v>90</v>
+      </c>
+      <c r="B69" t="s">
+        <v>19</v>
+      </c>
+      <c r="C69" t="s">
         <v>91</v>
-      </c>
-      <c r="B69" t="s">
-        <v>20</v>
-      </c>
-      <c r="C69" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -5512,817 +5507,817 @@
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B27">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C27">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B28">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C28">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B29">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C29">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B30">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C30">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B31">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C31">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B32">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C32">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B33">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C33">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B34">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C34">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B35">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C35">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B36">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C36">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B37">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C37">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B38">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C38">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B39">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C39">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B40">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C40">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B41">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C41">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B42">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C42">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B43">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C43">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B44">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C44">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B45">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C45">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B46">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C46">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B47">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C47">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B48">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C48">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B49">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C49">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B50">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C50">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B51">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C51">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B52">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C52">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B53">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C53">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B54">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C54">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B55">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C55">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B56">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C56">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B57">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C57">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B58">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C58">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B59">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C59">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B60">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C60">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B61">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C61">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B62">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C62">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B63">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C63">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B64">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C64">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B65">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C65">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B66">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C66">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B67">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C67">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B68">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C68">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B69">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C69">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B70">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C70">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B71">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C71">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B72">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C72">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B73">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C73">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B74">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C74">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B75">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C75">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B76">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C76">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B77">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C77">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B78">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C78">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B79">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C79">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B80">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C80">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B81">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C81">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B82">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C82">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B83">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C83">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B84">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C84">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B85">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C85">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B86">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C86">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B87">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C87">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B88">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C88">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B89">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C89">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B90">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C90">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B91">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C91">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B92">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C92">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B93">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C93">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B94">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C94">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B95">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C95">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B96">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C96">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B97">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C97">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B98">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C98">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B99">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C99">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B100">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C100">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B101">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C101">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B102">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C102">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B103">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C103">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B104">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C104">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B105">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C105">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B106">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C106">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B107">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C107">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B108">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C108">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B109">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C109">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B110">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C110">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B111">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C111">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B112">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C112">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B113">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C113">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B114">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C114">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B115">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C115">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B116">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C116">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B117">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C117">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B118">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C118">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B119">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C119">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B120">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C120">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B121">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C121">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B122">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C122">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B123">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C123">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B124">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C124">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B125">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C125">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B126">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C126">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B127">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C127">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B128">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C128">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B129">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C129">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B130">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C130">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B131">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C131">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B132">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C132">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B133">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C133">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B134">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C134">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B135">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C135">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B136">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C136">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B137">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C137">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B138">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C138">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B139">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C139">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B140">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C140">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B141">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C141">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B142">
+      <formula1>Categories!$C$2:$C$17</formula1>
+    </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C142">
       <formula1>0</formula1>
       <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B142">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C141">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B141">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C140">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B140">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C139">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B139">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C138">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B138">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C137">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B137">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C136">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B136">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C135">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B135">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C134">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B134">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C133">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B133">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C132">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B132">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C131">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B131">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C130">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B130">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C129">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B129">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C128">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B128">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C127">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B127">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C126">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B126">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C125">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B125">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C124">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B124">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C123">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B123">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C122">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B122">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C121">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B121">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C120">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B120">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C119">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B119">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C118">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B118">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C117">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B117">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C116">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B116">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C115">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B115">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C114">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B114">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C113">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B113">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C112">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B112">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C111">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B111">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C110">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B110">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C109">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B109">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C108">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B108">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C107">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B107">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C106">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B106">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C105">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B105">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C104">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B104">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C103">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B103">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C102">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B102">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C101">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B101">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C100">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B100">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C99">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B99">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C98">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B98">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C97">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B97">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C96">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B96">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C95">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B95">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C94">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B94">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C93">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B93">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C92">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B92">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C91">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B91">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C90">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B90">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C89">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B89">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C88">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B88">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C87">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B87">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C86">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B86">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C85">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B85">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C84">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B84">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C83">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B83">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C82">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B82">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C81">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B81">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C80">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B80">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C79">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B79">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C78">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B78">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C77">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B77">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C76">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B76">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C75">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B75">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C74">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B74">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C73">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B73">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C72">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B72">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C71">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B71">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C70">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B70">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C69">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B69">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C68">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B68">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C67">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B67">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C66">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B66">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C65">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B65">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C64">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B64">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C63">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B63">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C62">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B62">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C61">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B61">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C60">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B60">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C59">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B59">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C58">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B58">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C57">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B57">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C56">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B56">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C55">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B55">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C54">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B54">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C53">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B53">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C52">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B52">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C51">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B51">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C50">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B50">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C49">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B49">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C48">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B48">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C47">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B47">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C46">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B46">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C45">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B45">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C44">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B44">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C43">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B43">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C42">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B42">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C41">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B41">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C40">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B40">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C39">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B39">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C38">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B38">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C37">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B37">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C36">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B36">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C35">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B35">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C34">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B34">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C33">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B33">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C32">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B32">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C31">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B31">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C30">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B30">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C29">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B29">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C28">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B28">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C27">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B27">
-      <formula1>Categories!$C$2:$C$17</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions gridLines="false" gridLinesSet="true"/>
@@ -6358,7 +6353,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -6366,18 +6361,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4"/>
     </row>
@@ -6389,68 +6384,68 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10"/>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12"/>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14"/>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B17"/>
     </row>
@@ -6488,52 +6483,52 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -6570,7 +6565,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -7111,15 +7106,15 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" t="s">
         <v>106</v>
-      </c>
-      <c r="B1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7128,7 +7123,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3">
         <v>0</v>

</xml_diff>

<commit_message>
Actually updated files for use in real system, fixed small errors
</commit_message>
<xml_diff>
--- a/Templates/Template Hours Log.xlsx
+++ b/Templates/Template Hours Log.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="134">
   <si>
     <t>Time Report</t>
   </si>
@@ -64,9 +64,15 @@
     <t>Custom Services - Consulting and Training</t>
   </si>
   <si>
+    <t>Subcontract to David Evans Associates - DEA for scenario planning for BTPO</t>
+  </si>
+  <si>
     <t>Boston College ITEST</t>
   </si>
   <si>
+    <t>Custom Services - Consulting &amp; Training</t>
+  </si>
+  <si>
     <t>CAMPO NEAS</t>
   </si>
   <si>
@@ -76,9 +82,15 @@
     <t>CHARM GOMP</t>
   </si>
   <si>
+    <t>Gulf of Mexico Program CHARM project for Mississippi.</t>
+  </si>
+  <si>
     <t>CHARM-CACBI</t>
   </si>
   <si>
+    <t>Houston - CACBI project (CHARM, TCWP)</t>
+  </si>
+  <si>
     <t>CommunityViz Design 4.3</t>
   </si>
   <si>
@@ -163,6 +175,12 @@
     <t>GOMP Clip and Ship</t>
   </si>
   <si>
+    <t>Custom Services - Software</t>
+  </si>
+  <si>
+    <t>Gulf of Mexico Program-funded project for Texas Coastal Watershed Program, Steve Mikulencak.</t>
+  </si>
+  <si>
     <t>Holiday</t>
   </si>
   <si>
@@ -187,6 +205,9 @@
     <t>Michigan Energy Options</t>
   </si>
   <si>
+    <t>Online tool developed as sub to UCSB using SeaSketch technology</t>
+  </si>
+  <si>
     <t>M-NCPPC</t>
   </si>
   <si>
@@ -220,18 +241,21 @@
     <t>Seven Hills - Performance Enhancements</t>
   </si>
   <si>
-    <t>Custom Services - Software</t>
-  </si>
-  <si>
     <t>SEWRPC</t>
   </si>
   <si>
+    <t>CommunityViz for VISION 2050 by Southeastern Wisconsin Regional Planning Commission</t>
+  </si>
+  <si>
     <t>SLO Community Design Model</t>
   </si>
   <si>
     <t>SLOCOG SCS</t>
   </si>
   <si>
+    <t>Sustainable Communities Strategy for SLOCOG</t>
+  </si>
+  <si>
     <t>Testing:  CommunityViz 4.2</t>
   </si>
   <si>
@@ -283,6 +307,9 @@
     <t>UCSD Water Model</t>
   </si>
   <si>
+    <t>UCSD Spatial Analytical Tool Box - Phase I</t>
+  </si>
+  <si>
     <t>Unpaid Time Off</t>
   </si>
   <si>
@@ -310,18 +337,66 @@
     <t>New Products</t>
   </si>
   <si>
+    <t>Time Off</t>
+  </si>
+  <si>
     <t>{Names}</t>
   </si>
   <si>
+    <t>Anderson, Amy</t>
+  </si>
+  <si>
+    <t>Borchert, Thomas</t>
+  </si>
+  <si>
+    <t>Carr, Mike</t>
+  </si>
+  <si>
+    <t>Christensen, Eric</t>
+  </si>
+  <si>
     <t>Davis, Joel</t>
   </si>
   <si>
+    <t>Debay, Dennis</t>
+  </si>
+  <si>
+    <t>Flesche, Charlie</t>
+  </si>
+  <si>
+    <t>Gibson, Nicole</t>
+  </si>
+  <si>
+    <t>Gustin, Merix</t>
+  </si>
+  <si>
+    <t>Jerome, Mitch</t>
+  </si>
+  <si>
+    <t>Johnson, Aviva</t>
+  </si>
+  <si>
+    <t>Joynt, Erin</t>
+  </si>
+  <si>
     <t>Keating, Madeline</t>
   </si>
   <si>
     <t>Lewelling, Kelley</t>
   </si>
   <si>
+    <t>Meroney, Brett</t>
+  </si>
+  <si>
+    <t>Sanschagrin (Cubbon), Emily</t>
+  </si>
+  <si>
+    <t>Seidel, Erty</t>
+  </si>
+  <si>
+    <t>Smith (Berndt), Carisa</t>
+  </si>
+  <si>
     <t>Varley, Ian</t>
   </si>
   <si>
@@ -334,7 +409,7 @@
     <t>Walker, Mary</t>
   </si>
   <si>
-    <t>Williams, Katie</t>
+    <t>Woodward, Anne</t>
   </si>
   <si>
     <t>{Sundays}</t>
@@ -1377,7 +1452,7 @@
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <dataValidations count="2">
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose your name from this list" sqref="A3">
-      <formula1>People!$A$2:$A$10</formula1>
+      <formula1>People!$A$2:$A$31</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose your starting date from this list" sqref="A6">
       <formula1>Dates!$A$2:$A$85</formula1>
@@ -4340,285 +4415,293 @@
       <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D2"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C3"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5"/>
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6"/>
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C7"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C9"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
         <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
       </c>
       <c r="C10"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C11"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C12"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C13"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C14"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C16"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C17"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C19"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
         <v>39</v>
-      </c>
-      <c r="B21" t="s">
-        <v>35</v>
       </c>
       <c r="C21"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C22"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C23"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C25"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C26"/>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C27"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28"/>
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C29"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C30"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C31"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
         <v>12</v>
@@ -4627,7 +4710,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
         <v>12</v>
@@ -4636,7 +4719,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B34" t="s">
         <v>12</v>
@@ -4645,7 +4728,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B35" t="s">
         <v>12</v>
@@ -4654,16 +4737,18 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B36" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36"/>
+        <v>50</v>
+      </c>
+      <c r="C36" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B37" t="s">
         <v>12</v>
@@ -4672,7 +4757,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B38" t="s">
         <v>12</v>
@@ -4681,36 +4766,36 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C39"/>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C40"/>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B42" t="s">
         <v>12</v>
@@ -4719,52 +4804,54 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C43"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B44" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C44"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B45" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C45"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C46"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>12</v>
-      </c>
-      <c r="C47"/>
+        <v>15</v>
+      </c>
+      <c r="C47" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B48" t="s">
         <v>12</v>
@@ -4773,61 +4860,63 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B49" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49"/>
+        <v>15</v>
+      </c>
+      <c r="C49" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B50" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C50"/>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B51" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C51"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B52" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C52"/>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B53" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C53"/>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B54" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C54"/>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B55" t="s">
         <v>12</v>
@@ -4836,7 +4925,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B56" t="s">
         <v>12</v>
@@ -4845,7 +4934,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B57" t="s">
         <v>12</v>
@@ -4854,16 +4943,16 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B58" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C58"/>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B59" t="s">
         <v>12</v>
@@ -4872,7 +4961,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B60" t="s">
         <v>12</v>
@@ -4881,7 +4970,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B61" t="s">
         <v>12</v>
@@ -4890,78 +4979,80 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B62" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C62" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B63" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C63"/>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B64" t="s">
-        <v>12</v>
-      </c>
-      <c r="C64"/>
+        <v>15</v>
+      </c>
+      <c r="C64" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B65" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C65"/>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B66" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C66"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B67" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C67"/>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B68" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C68"/>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B69" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C69" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -5337,987 +5428,987 @@
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B2">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B3">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C3">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B4">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C4">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B5">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C5">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B6">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C6">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B7">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C7">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B8">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C8">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B9">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C9">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B10">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C10">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B11">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C11">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B12">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C12">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B13">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C13">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B14">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C14">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B15">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C15">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B16">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C16">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B17">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C17">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B18">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C18">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B19">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C19">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B20">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C20">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B21">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C21">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B22">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C22">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B23">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C23">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B24">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C24">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B25">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C25">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B26">
-      <formula1>Categories!$C$2:$C$17</formula1>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C26">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C142">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B142">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C141">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B141">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C140">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B140">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C139">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B139">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C138">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B138">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C137">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B137">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C136">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B136">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C135">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B135">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C134">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B134">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C133">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B133">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C132">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B132">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C131">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B131">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C130">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B130">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C129">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B129">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C128">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B128">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C127">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B127">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C126">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B126">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C125">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B125">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C124">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B124">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C123">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B123">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C122">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B122">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C121">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B121">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C120">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B120">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C119">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B119">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C118">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B118">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C117">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B117">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C116">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B116">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C115">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B115">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C114">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B114">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C113">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B113">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C112">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B112">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C111">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B111">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C110">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B110">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C109">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B109">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C108">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B108">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C107">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B107">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C106">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B106">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C105">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B105">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C104">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B104">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C103">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B103">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C102">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B102">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C101">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B101">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C100">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B100">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C99">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B99">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C98">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B98">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C97">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B97">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C96">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B96">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C95">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B95">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C94">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B94">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C93">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B93">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C92">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B92">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C91">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B91">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C90">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B90">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C89">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B89">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C88">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B88">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C87">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B87">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C86">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B86">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C85">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B85">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C84">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B84">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C83">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B83">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C82">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B82">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C81">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B81">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C80">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B80">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C79">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B79">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C78">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B78">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C77">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B77">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C76">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B76">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C75">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B75">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C74">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B74">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C73">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B73">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C72">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B72">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C71">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B71">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C70">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B70">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C69">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B69">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C68">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B68">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C67">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B67">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C66">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B66">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C65">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B65">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C64">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B64">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C63">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B63">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C62">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B62">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C61">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B61">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C60">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B60">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C59">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B59">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C58">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B58">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C57">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B57">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C56">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B56">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C55">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B55">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C54">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B54">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C53">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B53">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C52">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B52">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C51">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B51">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C50">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B50">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C49">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B49">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C48">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B48">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C47">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B47">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C46">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B46">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C45">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B45">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C44">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B44">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C43">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B43">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C42">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B42">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C41">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B41">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C40">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B40">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C39">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B39">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C38">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B38">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C37">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B37">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C36">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B36">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C35">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B35">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C34">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B34">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C33">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B33">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C32">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B32">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C31">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B31">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C30">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B30">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C29">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B29">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C28">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B28">
+      <formula1>Categories!$C$2:$C$27</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C27">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B27">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C27">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B28">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C28">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B29">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C29">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B30">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C30">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B31">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C31">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B32">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C32">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B33">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C33">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B34">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C34">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B35">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C35">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B36">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C36">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B37">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C37">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B38">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C38">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B39">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C39">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B40">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C40">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B41">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C41">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B42">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C42">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B43">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C43">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B44">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C44">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B45">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C45">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B46">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C46">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B47">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C47">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B48">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C48">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B49">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C49">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B50">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C50">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B51">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C51">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B52">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C52">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B53">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C53">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B54">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C54">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B55">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C55">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B56">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C56">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B57">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C57">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B58">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C58">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B59">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C59">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B60">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C60">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B61">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C61">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B62">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C62">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B63">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C63">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B64">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C64">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B65">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C65">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B66">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C66">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B67">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C67">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B68">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C68">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B69">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C69">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B70">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C70">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B71">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C71">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B72">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C72">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B73">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C73">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B74">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C74">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B75">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C75">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B76">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C76">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B77">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C77">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B78">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C78">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B79">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C79">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B80">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C80">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B81">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C81">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B82">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C82">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B83">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C83">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B84">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C84">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B85">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C85">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B86">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C86">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B87">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C87">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B88">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C88">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B89">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C89">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B90">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C90">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B91">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C91">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B92">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C92">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B93">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C93">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B94">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C94">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B95">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C95">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B96">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C96">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B97">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C97">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B98">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C98">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B99">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C99">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B100">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C100">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B101">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C101">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B102">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C102">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B103">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C103">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B104">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C104">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B105">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C105">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B106">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C106">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B107">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C107">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B108">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C108">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B109">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C109">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B110">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C110">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B111">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C111">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B112">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C112">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B113">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C113">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B114">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C114">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B115">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C115">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B116">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C116">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B117">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C117">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B118">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C118">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B119">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C119">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B120">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C120">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B121">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C121">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B122">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C122">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B123">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C123">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B124">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C124">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B125">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C125">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B126">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C126">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B127">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C127">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B128">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C128">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B129">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C129">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B130">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C130">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B131">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C131">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B132">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C132">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B133">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C133">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B134">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C134">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B135">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C135">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B136">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C136">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B137">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C137">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B138">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C138">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B139">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C139">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B140">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C140">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B141">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C141">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Choose a category from this list" sqref="B142">
-      <formula1>Categories!$C$2:$C$17</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="stop" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Only numbers between 0 and 24 are allowed!" promptTitle="Allowed input" prompt="Only numbers between 0 and 24 are allowed." sqref="C142">
-      <formula1>0</formula1>
-      <formula2>24</formula2>
+      <formula1>Categories!$C$2:$C$27</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions gridLines="false" gridLinesSet="true"/>
@@ -6339,7 +6430,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="B12" sqref="B12"/>
@@ -6353,7 +6444,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -6361,93 +6452,154 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>93</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="B2"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="B3"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B4"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B5"/>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>82</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B6"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="B7"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>65</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B8"/>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9"/>
+        <v>90</v>
+      </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="B10"/>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>94</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="B11"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B12"/>
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>19</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B13"/>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="B14"/>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>37</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B15"/>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B16"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B17"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -6470,7 +6622,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A31"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A8" sqref="A8"/>
@@ -6483,52 +6635,157 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -6565,7 +6822,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -7106,15 +7363,15 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7123,7 +7380,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="B3">
         <v>0</v>

</xml_diff>